<commit_message>
fix get id in dom
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -11,6 +11,8 @@
     <sheet name="all1726300902724" sheetId="6" r:id="rId6"/>
     <sheet name="me-be1726330049414" sheetId="7" r:id="rId7"/>
     <sheet name="all1726330049590" sheetId="8" r:id="rId8"/>
+    <sheet name="sua-cho-be1726453966878" sheetId="9" r:id="rId9"/>
+    <sheet name="all1726453966983" sheetId="10" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
@@ -993,6 +995,220 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>url</v>
+      </c>
+      <c r="C1" t="str">
+        <v>title</v>
+      </c>
+      <c r="D1" t="str">
+        <v>type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>inventoryQuantity</v>
+      </c>
+      <c r="F1" t="str">
+        <v>inventoryPolicy</v>
+      </c>
+      <c r="G1" t="str">
+        <v>sku</v>
+      </c>
+      <c r="H1" t="str">
+        <v>barcode</v>
+      </c>
+      <c r="I1" t="str">
+        <v>featuredImage</v>
+      </c>
+      <c r="J1" t="str">
+        <v>images</v>
+      </c>
+      <c r="K1" t="str">
+        <v>trademark</v>
+      </c>
+      <c r="L1" t="str">
+        <v>shortDescription</v>
+      </c>
+      <c r="M1" t="str">
+        <v>price</v>
+      </c>
+      <c r="N1" t="str">
+        <v>originalPrice</v>
+      </c>
+      <c r="O1" t="str">
+        <v>percentDiscount</v>
+      </c>
+      <c r="P1" t="str">
+        <v>description</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1055411201</v>
+      </c>
+      <c r="B2" t="str">
+        <v>https://sakukostore.com.vn/products/sachi-mochi-mochi-vi-cam-nhat-200g</v>
+      </c>
+      <c r="C2" t="str">
+        <v>SACHI MOCHI- Mochi vị cam Nhật 200g</v>
+      </c>
+      <c r="D2" t="str">
+        <v>BÁNH KẸO, ĐỒ ĂN VẶT</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <v>deny</v>
+      </c>
+      <c r="G2" t="str">
+        <v>153314</v>
+      </c>
+      <c r="H2" t="str">
+        <v>4971679301063</v>
+      </c>
+      <c r="I2" t="str">
+        <v>https://product.hstatic.net/200000833669/product/vi_cam_ff5c0af7b11c46609b460cb9e85d9f47.png</v>
+      </c>
+      <c r="J2" t="str">
+        <v>https://product.hstatic.net/200000833669/product/vi_cam_ff5c0af7b11c46609b460cb9e85d9f47.png</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Khác</v>
+      </c>
+      <c r="L2" t="str">
+        <v>SACHI MOCHI- Mochi vị cam Nhật 200g</v>
+      </c>
+      <c r="M2">
+        <v>11500000</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="str">
+        <v>0%</v>
+      </c>
+      <c r="P2" t="str">
+        <v>SACHI MOCHI- Mochi vị cam Nhật 200g</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1052913902</v>
+      </c>
+      <c r="B3" t="str">
+        <v>https://sakukostore.com.vn/products/seiki-banh-mochi-daifuku-vi-dua-luoi-30-cai</v>
+      </c>
+      <c r="C3" t="str">
+        <v>[TRUNG THU 2024] SEIKI- Bánh Mochi Daifuku vị dưa lưới 30 cái</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Bánh</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3" t="str">
+        <v>continue</v>
+      </c>
+      <c r="G3" t="str">
+        <v>153238</v>
+      </c>
+      <c r="H3" t="str">
+        <v>4990485004982</v>
+      </c>
+      <c r="I3" t="str">
+        <v>https://product.hstatic.net/200000833669/product/4990485004982_1_c8f96ded3e4b4345bfaa6636365d0698.jpg</v>
+      </c>
+      <c r="J3" t="str">
+        <v>https://product.hstatic.net/200000833669/product/4990485004982_1_c8f96ded3e4b4345bfaa6636365d0698.jpg,https://product.hstatic.net/200000833669/product/4990485004982_2_d3b03b2d62f34ec1a0357b4c8b02ab2a.jpeg</v>
+      </c>
+      <c r="K3" t="str">
+        <v>SEIKI</v>
+      </c>
+      <c r="L3" t="str">
+        <v>Vỏ bánh từ gạo mochi cao cấp mềm dẻoNhân kem dưa lưới thơm mátPhù hợp thưởng thức cùng trà nóng</v>
+      </c>
+      <c r="M3">
+        <v>29250000</v>
+      </c>
+      <c r="N3">
+        <v>32500000</v>
+      </c>
+      <c r="O3" t="str">
+        <v>10%</v>
+      </c>
+      <c r="P3" t="str">
+        <v>&lt;div class="section-title text-blue"&gt;&lt;h1&gt;&lt;strong&gt;TRUNG THU VIỆT, CHỌN VỊ NHẬT&lt;/strong&gt;&lt;/h1&gt;&lt;p&gt;Trải qua hàng nghìn năm lịch sử, những chiếc bánh&amp;nbsp;Nhật Bản đã trở thành biểu tượng của nghệ thuật và văn hóa ẩm thực độc đáo, sở hữu một hương vị riêng không lẫn vào đâu được. Bất kỳ ai cũng&amp;nbsp;chẳng thể cưỡng lại sự quyến rũ từ vị ngọt dịu dàng, sự hòa quyện giữa hương vị truyền thống và hiện đại. Nguyên liệu sử dụng cho việc chế biến đều được xứ sở hoa anh đào gửi gắm rất nhiều tình cảm và công phu.&lt;/p&gt;&lt;p&gt;Mùa Trung Thu năm nay, Sakuko đem đến cho quý khách hàng cơ hội để có thể trải nghiệm những thức quà đậm nét văn hóa Nhật Bản, thông qua những chiếc bánh Mochi hay Daifuku. Hãy đặt hàng ngay để không bỏ lỡ ưu đãi lên tới 40% cùng hương vị khó quên.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;THỜI GIAN NHẬN ĐẶT HÀNG: 11/06/2024&amp;nbsp;- 25/06/2024&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;THỜI ĐIỂM DỰ KIẾN HÀNG VỀ: 12/09/2024&lt;/strong&gt;&lt;/p&gt;&lt;p style="text-align: center"&gt;&lt;img style="width: 847.988px; height: 443.984px;" src="//file.hstatic.net/200000833669/file/sakuko_2400x1256_mochi_11062024_0568fb6fd5b44f91a0b2168c3ba6c2bb_grande.jpg"&gt;&lt;/p&gt;Thông tin sản phẩm&lt;/div&gt;&lt;div class="article-content show-hide-content"&gt;&lt;div&gt;&lt;strong&gt;TÊN SP&lt;/strong&gt; : SEIKI- Bánh Mochi Daifuku vị dưa lưới 30 cái&lt;p&gt;&lt;strong&gt;KHỐI LƯỢNG TỊNH&lt;/strong&gt; : 360g/ hộp (30 cái)&lt;/p&gt;&lt;p&gt;&lt;strong&gt;HSD&lt;/strong&gt; : Xem trên bao bì sản phẩm&lt;/p&gt;&lt;p&gt;&lt;strong&gt;NGÀY SX&lt;/strong&gt; : Trước HSD 6 tháng&lt;/p&gt;&lt;p&gt;&lt;strong&gt;THÀNH PHẦN&lt;/strong&gt; : Xi-rô tinh bột (sản xuất tại Nhật Bản), đường, bột gạo nếp, tinh bột, dầu thực vật, lactose, sữa bột nguyên chất, bột kem, bơ ca cao, bột whey, dưa xay nhuyễn, xi-rô đảo đường/trehalose, chất nhũ hoá, hương liệu tổng hợp, phẩm màu tự nhiên (carotenoid)&lt;/p&gt;&lt;p&gt;&lt;strong&gt;CÔNG DỤNG&lt;/strong&gt; : Bánh mochi truyền thống Nhật Bản với vỏ bánh mềm thơm, nhân dưa lưới hấp dẫn.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;THÔNG TIN CẢNH BÁO&lt;/strong&gt; : Không sử dụng sản phẩm quá hạn. Lưu ý thành phần dị ứng&lt;/p&gt;&lt;p&gt;&lt;strong&gt;HDSD&lt;/strong&gt; : Ăn trực tiếp.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;BẢO QUẢN&lt;/strong&gt; : Tránh ánh nắng trực tiếp, nhiệt độ cao và độ ẩm&lt;/p&gt;&lt;p&gt;&lt;strong&gt;NHÀ SX&lt;/strong&gt; : Seiki Co.,Ltd.; 1240-1 Kitagawara, Matsumae-machi, Iyo-gun, Ehime, Nhật Bản.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;XUẤT XỨ&lt;/strong&gt; : Nhật Bản&lt;/p&gt;&lt;p&gt;&lt;strong&gt;CODE&lt;/strong&gt; : 4990485004982&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Số CB&lt;/strong&gt; : 132/BJ/2023&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>1052890607</v>
+      </c>
+      <c r="B4" t="str">
+        <v>https://sakukostore.com.vn/products/sua-meiji-so-0-1-tuoi-dang-hop-sat</v>
+      </c>
+      <c r="C4" t="str">
+        <v>MEIJI- Sữa số 0 cho bé từ 0-1 tuổi 800g</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Sữa Meiji</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4" t="str">
+        <v>continue</v>
+      </c>
+      <c r="G4" t="str">
+        <v>150458</v>
+      </c>
+      <c r="H4" t="str">
+        <v>4902705116542</v>
+      </c>
+      <c r="I4" t="str">
+        <v>https://product.hstatic.net/200000833669/product/meiji-suaso0chobetu0-1tuoi800g_dd28e4aa93e54376b54bc080999738c0.png</v>
+      </c>
+      <c r="J4" t="str">
+        <v>https://product.hstatic.net/200000833669/product/meiji-suaso0chobetu0-1tuoi800g_dd28e4aa93e54376b54bc080999738c0.png</v>
+      </c>
+      <c r="K4" t="str">
+        <v>MEIJI</v>
+      </c>
+      <c r="L4" t="str">
+        <v>Sữa Meiji số 0 - 1 tuổi dạng hộp sắt có hương vị gần giống sữa mẹ, giúp bé dễ thích nghi, không chê ti mẹ cùng thành phần chất xơ tự nhiên tránh táo bón.</v>
+      </c>
+      <c r="M4">
+        <v>48500000</v>
+      </c>
+      <c r="N4">
+        <v>55500000</v>
+      </c>
+      <c r="O4" t="str">
+        <v>12.612612612612612%</v>
+      </c>
+      <c r="P4" t="str">
+        <v>&lt;h2 class="section-title text-blue"&gt;&lt;span style="color:#ff0066"&gt;&lt;strong&gt;Thông số sản phẩm&lt;/strong&gt;&lt;/span&gt;&lt;/h2&gt;&lt;div class="data-table"&gt;&lt;table&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td&gt;&lt;span&gt;Sản phẩm&lt;/span&gt;&lt;/td&gt;&lt;td&gt;&lt;span&gt;Sữa Meiji số 0-1 tuổi&lt;/span&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;span&gt;Xuất xứ&lt;/span&gt;&lt;/td&gt;&lt;td&gt;&lt;span&gt;Nhật Bản&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;span&gt;Hãng sản xuất&lt;/span&gt;&lt;/td&gt;&lt;td&gt;&lt;span&gt;Meiji&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;span&gt;Trọng lượng&lt;/span&gt;&lt;/td&gt;&lt;td&gt;&lt;span&gt;800g&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;span&gt;Quy cách đóng gói&lt;/span&gt;&lt;/td&gt;&lt;td&gt;&lt;span&gt;Hộp sẳt&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;div&gt;&amp;nbsp;&lt;/div&gt;&lt;/div&gt;&lt;div class="section-title text-blue"&gt;&lt;strong&gt;Thông tin sản phẩm&lt;/strong&gt;&lt;/div&gt;&lt;div class="article-content show-hide-content"&gt;&lt;p&gt;&lt;strong&gt;Sữa Meiji số 0 - 1 tuổi dạng hộp sắt&lt;/strong&gt; là sữa bột công thức hàng đầu cho trẻ sơ sinh được các mẹ bỉm sữa nội địa Nhật và cả Việt Nam tin dùng. Bởi sữa Meiji số 0 có hương vị gần giống sữa mẹ, giúp bé dễ thích nghi với sữa bột, lại không chê ti mẹ. Đặc biệt, sữa có thành phần bổ sung chất xơ tự nhiên hạn chế bị táo bón hiệu quả.&lt;/p&gt;&lt;h2&gt;&lt;strong&gt;1. Thành phần dinh dưỡng sữa Meiji số 0&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;&lt;img alt="Bảng thành phần dinh dưỡng của sữa Meiji số 0" title="Bảng thành phần dinh dưỡng của sữa Meiji số 0" src="https://product.hstatic.net/200000833669/product/bang-dinh-duong-sua-meiji-so-0-1-tuoi_8e2ded54f4dc45559f2f45ecd320b440.jpg"&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Bảng dinh dưỡng sữa Meiji số 0 cho bé 0 - 12 tháng tuổi&lt;/em&gt;&lt;/p&gt;&lt;h2&gt;&lt;strong&gt;2. Thành phần nổi bật&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;Sữa Meiji số 0 hỗ trợ mẹ mang đến cho bé nguồn dinh dưỡng an toàn, đầy đủ để vững tin phát triển trong những năm tháng đầu đời. Cụ thể, sữa Meiji có những thành phần nổi bật đó là:&lt;/p&gt;&lt;h3&gt;Bổ sung chất xơ tự nhiên FOS (Fructo-Oligosaccharides)&lt;/h3&gt;&lt;p&gt;Các nghiên cứu cho thấy FOS là chất xơ hòa tan, có rất nhiều lợi ích đối với sức khỏe con người. Đây là người bạn tuyệt vời của hệ tiêu hóa, tim mạch, hệ miễn dịch,...&lt;/p&gt;&lt;h3&gt;Cung cấp nhiều vitamin và các khoáng chất thiết yếu&lt;/h3&gt;&lt;p&gt;Trong thành phần của sữa Meiji rất giàu vitamin như: A, C, D, vitamin nhóm B,... cùng các khoáng chất cần thiết (sắt, kẽm, photpho,...) hỗ trợ tối ưu sự phát triển toàn diện cho bé.&lt;/p&gt;&lt;h3&gt;Bổ sung các Nucleotides tự nhiên có trong sữa mẹ&lt;/h3&gt;&lt;p&gt;Meiji hiểu rằng ở giai đoạn đầu đời hệ miễn dịch của con còn rất non yếu, dễ bị vi khuẩn tấn công và nhiễm bệnh. Vì thế, công thức sữa cho trẻ sơ sinh của Meiji đã bổ sung thêm các Nucleotides tự nhiên có trong sữa mẹ giúp tăng cường đề kháng.&lt;/p&gt;&lt;p&gt;&lt;img src="https://product.hstatic.net/200000833669/product/se1bbafa-meiji-0-2_16b8a8ff0726471c9a9833f51053862b.jpg"&gt;&lt;img src="https://product.hstatic.net/200000833669/product/se1bbafa-meiji-0_3da58f5faf6c4823b559a5d1ecdd4674.jpg"&gt;&lt;/p&gt;&lt;div&gt;&lt;div class="ace-line ace-line old-record-id-WDu1dC4sBowBjSxZhEDlYiHSgrh"&gt;&lt;em&gt;Thiết kế bao bì dễ sử dụng của sữa Meiji số 0 nội địa Nhật&lt;/em&gt;&lt;/div&gt;&lt;/div&gt;&lt;h2&gt;&lt;strong&gt;3. Đặc điểm nổi bật của sữa Meiji số 0&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;Cẩm nang nuôi con khỏe mạnh - thông minh của nhiều mẹ bỉm sữa chia sẻ thường dành nhiều lời khen ngợi cho sữa Meiji số 0. Bởi sản phẩm có những đặc điểm nổi bật mà mẹ rất tâm đắc, cụ thể:&lt;/p&gt;&lt;h3&gt;Sữa có vị nhạt, mùi vị gần giống sữa mẹ&lt;/h3&gt;&lt;p&gt;Các mẹ thường có một nỗi lo lắng chung là sữa công thức thơm ngon hơn sữa mẹ, dễ khiến bé chê ti mẹ. Trong khi đó, sữa mẹ luôn là nguồn dinh dưỡng tốt nhất cho sự phát triển của trẻ sơ sinh và trẻ nhỏ. Hiểu được điều đó, sữa Meiji số 0 đã ra đời với hương thơm cùng mùi vị gần giống sữa mẹ nhất. Do vậy, mẹ cứ yên tâm sử dụng cả sữa mẹ lẫn sữa công thức cho bé nhé!&lt;/p&gt;&lt;h3&gt;Hỗ trợ bé tăng cân, chiều cao đều, không tăng nhanh, tránh béo phì&lt;/h3&gt;&lt;p&gt;Với thành phần dinh dưỡng cân bằng, hướng tới sự phát triển toàn diện, sữa Meiji số 0 là người bạn đồng hành lý tưởng hỗ trợ bé tăng cân và chiều cao đồng đều. Nhờ vậy, mẹ chẳng lo con bị béo phì, thừa cân mà có thể yên tâm nhìn con cao lớn từng chút một khỏe mạnh và ổn định.&lt;/p&gt;&lt;p&gt;&lt;img alt="Sữa Meiji số 0 giúp bé hạn chế táo bón" title="Sữa Meiji số 0 giúp bé hạn chế táo bón" src="https://product.hstatic.net/200000833669/product/sua-meiji-so-0-giup-be-han-che-tao-bon_ba6b62df8c574dacbd09e603cbf5624c.jpg"&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Với sữa Meiji số 0 mẹ có thể an tâm con tiêu hóa tốt, ít bị táo bón&lt;span&gt;&amp;nbsp;&lt;/span&gt;&lt;/em&gt;&lt;/p&gt;&lt;h3&gt;Hạn chế táo bón, phân xốp cùng hệ tiêu hóa khỏe mạnh&lt;/h3&gt;&lt;p&gt;Sữa Meiji giúp bé củng cố sức khỏe đường ruột, tiêu hóa tốt hơn nhờ có thành phần chất xơ tự nhiên FOS. Bởi khi vào ruột, FOS sẽ hút nước trương nở tạo khối phân, làm mềm phân và giúp đào thải phân cùng các chất cặn bã nhanh chóng ra khỏi cơ thể.&lt;/p&gt;&lt;p&gt;Bên cạnh đó, FOS còn có tác dụng&lt;strong&gt; kích thích các lợi khuẩn trong đường ruột phát triển&lt;/strong&gt;, đồng thời giúp tăng cường hấp thu canxi cùng magie tại ruột già. Vì thế, bé uống sữa Meiji mẹ yên tâm lắm bởi bé ít bị táo bón và hấp thu dưỡng chất tốt hơn.&lt;/p&gt;&lt;h3&gt;Tăng cường sức đề kháng, nâng cao miễn dịch&lt;/h3&gt;&lt;p&gt;Chất xơ hòa tan FOS cùng với &lt;strong&gt;các Nucleotides tự nhiên&lt;/strong&gt; trong sữa Meiji có khả năng tăng cường miễn dịch, cho bé sức đề kháng tốt để chống chọi với vi khuẩn, bệnh tật.&lt;/p&gt;&lt;h2&gt;&lt;strong&gt;4. Hướng dẫn cách pha sữa Meiji số 0&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;Nhiều mẹ bỉm sữa, nhất là những chị em làm mẹ lần đầu rất lúng túng trong việc pha sữa Meiji cho bé. Mẹ không biết 1 gạt thìa sữa pha khoảng bao nhiêu ml thì hợp lý. Dưới đây là hướng dẫn cách pha chuẩn theo hướng dẫn của nhà sản xuất các mẹ cần biết:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Một thìa gạt ngang&lt;/strong&gt; sữa Meiji tương đương 2,7g bột sữa pha được&lt;strong&gt; 20ml sữa.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Cách pha:&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bước 1: Đầu tiên, bố mẹ cần đun sôi dụng cụ pha sữa trong vòng&lt;strong&gt; 3 - 5 phút&lt;/strong&gt; để khử trùng.&lt;/li&gt;&lt;li&gt;Bước 2: Lấy nước sôi&lt;strong&gt; để&lt;/strong&gt; &lt;strong&gt;nguội đến 70 độ C&lt;/strong&gt; pha sữa.&lt;/li&gt;&lt;li&gt;Bước 3: Sử dụng thìa lấy sữa chuyên dụng trong hộp để lấy chính xác lượng sữa cần pha. Cho sữa vào dụng cụ pha rồi đổ vào &lt;strong&gt;⅔ lượng nước cần thiết&lt;/strong&gt; và lắc/ khuấy đều đến khi hòa tan sữa. (Do nước ở 70 độ C khá nóng nên bố mẹ cần cẩn thận tránh bị bỏng).&lt;/li&gt;&lt;li&gt;Bước 4: Đổ tiếp nước 70 độ vào bình cho đủ lượng nước theo chỉ định và tiếp tục lắc/ khuấy đều.&lt;/li&gt;&lt;li&gt;Bước 5: Chờ sữa nguội khoảng &lt;strong&gt;38 độ C&lt;/strong&gt; thì cho bé bú.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Tham khảo:&amp;nbsp;&lt;a style="font-family: -apple-system, BlinkMacSystemFont, 'Segoe UI', Roboto, 'Helvetica Neue', Arial, 'Noto Sans', sans-serif, 'Apple Color Emoji', 'Segoe UI Emoji', 'Segoe UI Symbol', 'Noto Color Emoji'; font-size: 1.25rem; font-weight: 700; background-color: #ffffff; text-align: left;" href="/blogs/me-be/huong-dan-cach-pha-sua-meiji-so-0-9-chuan"&gt;&lt;span&gt;[HƯỚNG DẪN] Cách pha sữa Meiji số 0, 9 chuẩn hướng dẫn Nhà sản xuất&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;div style="outline: 0px; vertical-align: baseline; margin: 0px; border-width: 0px 0px 1px; border-top-style: initial; border-right-style: initial; border-bottom-style: solid; border-left-style: initial; border-top-color: initial; border-right-color: initial; border-bottom-color: #ebebeb; border-left-color: initial; border-image: initial; padding: 0px 0px 15px; font-variant-numeric: inherit; font-variant-east-asian: inherit; font-variant-alternates: inherit; font-variant-position: inherit; font-stretch: inherit; line-height: inherit; font-family: -apple-system, BlinkMacSystemFont, 'Segoe UI', Roboto, 'Helvetica Neue', Arial, 'Noto Sans', sans-serif, 'Apple Color Emoji', 'Segoe UI Emoji', 'Segoe UI Symbol', 'Noto Color Emoji'; font-optical-sizing: inherit; font-kerning: inherit; font-feature-settings: inherit; font-variation-settings: inherit; display: flex; -webkit-box-pack: justify; justify-content: space-between; -webkit-box-align: center; align-items: center; color: #333333;" class="news-detail-meta flex justify-between items-center"&gt;&amp;nbsp;&lt;/div&gt;&lt;p&gt;&lt;img alt="Pha sữa Meiji số 0 dùng nước 70 độ " title="Pha sữa Meiji số 0 dùng nước 70 độ " src="https://product.hstatic.net/200000833669/product/pha-sua-meiji-so-0_6192ae5cb53d48f7ac4e3ab0b0c52cb4.jpg"&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Sữa Meiji số 0 khác với các loại sữa Nhật khác là sử dụng nước pha ở 70 độ C&lt;span&gt;&amp;nbsp;&lt;/span&gt;&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Mẹo khi pha sữa:&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Mẹ có thể&lt;strong&gt; cho bình sữa vào chậu nước mát, lạnh&lt;/strong&gt; để nguội nhanh hơn, tiết kiệm thời gian.&lt;/li&gt;&lt;li&gt;Trước khi cho bé bú, mẹ hãy &lt;strong&gt;kiểm tra nhiệt độ của sữa&lt;/strong&gt; tránh làm bỏng bé.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Liều lượng sữa cho bé theo từng độ tuổi:&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;img alt="Liều lượng sữa Meiji số 0 cho bé theo độ tuổi" title="Liều lượng sữa Meiji số 0 cho bé theo độ tuổi" src="https://product.hstatic.net/200000833669/product/lieu-luong-sua-meiji-so-0-theo-do-tuoi-cua-be_5ed9bd72449947e3bd19ac0f1138e626.jpg"&gt;&lt;/p&gt;&lt;p&gt;&lt;span&gt;&lt;em&gt;Tùy độ tuổi, cân nặng của bé mà mẹ sử dụng lượng sữa khác nhau&lt;/em&gt;&lt;/span&gt;&lt;span&gt;&lt;em&gt;&amp;nbsp;&lt;/em&gt;&lt;/span&gt;&lt;/p&gt;&lt;h2&gt;&lt;strong&gt;5. Hướng dẫn bảo quản&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;Mẹ cần chú ý bảo quản sữa đúng cách như sau:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bảo quản sữa Meiji ở những nơi khô thoáng&lt;/li&gt;&lt;li&gt;Tránh sự tiếp xúc với ánh nắng trực tiếp, những nơi có nhiệt độ cao hoặc ẩm ướt&lt;/li&gt;&lt;li&gt;Sữa Meiji đã pha có thời gian sử dụng là 2 tiếng sau khi pha và chỉ dùng 1 lần. Nếu bé uống không hết, còn thừa mẹ cũng tuyệt đối không cho bé dùng tiếp.&lt;/li&gt;&lt;li&gt;Hạn sử dụng của sữa được in dưới đáy lon là 18 tháng kể từ ngày sản xuất.&lt;/li&gt;&lt;li&gt;Đóng nắp sữa thật chặt sau mỗi lần lấy và chỉ nên sử dụng trong khoảng 30 ngày kể từ khi mở nắp hộp để đảm bảo chất lượng sữa tốt nhất. Sau 30 ngày sữa còn mẹ cũng có thể dụng nhưng chất lượng không bằng ban đầu.&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;&lt;strong&gt;6. Thông tin thương hiệu sữa Meiji&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;Sữa Meiji là sản phẩm của công ty Meiji thuộc tập đoàn Meiji Holdings Co., Ltd được thành lập vào năm 1917. Với tuổi đời hơn 100 năm, cái tên Meiji đã trở thành một trong những thương hiệu sữa truyền thống hàng đầu không chỉ ở Nhật Bản mà cả Châu Á. Các sản phẩm sữa của hãng luôn đảm bảo chất lượng tốt, đạt chứng nhận ISO 9001 được người dùng tại nhiều nước trên thế giới tin dùng.&lt;/p&gt;&lt;p&gt;Hiện Meiji cung cấp hơn 4000 mặt hàng với 6 dòng sản phẩm chính, chủ yếu là sản phẩm từ sữa. Trong đó, sữa bột, sữa chua,... chiếm thị phần số 1 ở thị trường nội địa Nhật.&lt;/p&gt;&lt;p&gt;Tại Việt Nam, sữa Meiji cũng nhận được nhiều đánh giá, review tốt của các mẹ bỉm sữa. Với chất lượng đảm bảo, tốt cho sự phát triển của bé và mức giá không quá cao, &lt;strong&gt;sữa Meiji số 0 - 1 tuổi dạng hộp sắt&lt;/strong&gt; vẫn luôn là sự lựa chọn hàng đầu cho giai đoạn đầu đời của bé.&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:P4"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P9"/>
@@ -4828,4 +5044,118 @@
     <ignoredError numberStoredAsText="1" sqref="A1:P13"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>url</v>
+      </c>
+      <c r="C1" t="str">
+        <v>title</v>
+      </c>
+      <c r="D1" t="str">
+        <v>type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>inventoryQuantity</v>
+      </c>
+      <c r="F1" t="str">
+        <v>inventoryPolicy</v>
+      </c>
+      <c r="G1" t="str">
+        <v>sku</v>
+      </c>
+      <c r="H1" t="str">
+        <v>barcode</v>
+      </c>
+      <c r="I1" t="str">
+        <v>featuredImage</v>
+      </c>
+      <c r="J1" t="str">
+        <v>images</v>
+      </c>
+      <c r="K1" t="str">
+        <v>trademark</v>
+      </c>
+      <c r="L1" t="str">
+        <v>shortDescription</v>
+      </c>
+      <c r="M1" t="str">
+        <v>price</v>
+      </c>
+      <c r="N1" t="str">
+        <v>originalPrice</v>
+      </c>
+      <c r="O1" t="str">
+        <v>percentDiscount</v>
+      </c>
+      <c r="P1" t="str">
+        <v>description</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1052890607</v>
+      </c>
+      <c r="B2" t="str">
+        <v>https://sakukostore.com.vn/products/sua-meiji-so-0-1-tuoi-dang-hop-sat</v>
+      </c>
+      <c r="C2" t="str">
+        <v>MEIJI- Sữa số 0 cho bé từ 0-1 tuổi 800g</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Sữa Meiji</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+      <c r="F2" t="str">
+        <v>continue</v>
+      </c>
+      <c r="G2" t="str">
+        <v>150458</v>
+      </c>
+      <c r="H2" t="str">
+        <v>4902705116542</v>
+      </c>
+      <c r="I2" t="str">
+        <v>https://product.hstatic.net/200000833669/product/meiji-suaso0chobetu0-1tuoi800g_dd28e4aa93e54376b54bc080999738c0.png</v>
+      </c>
+      <c r="J2" t="str">
+        <v>https://product.hstatic.net/200000833669/product/meiji-suaso0chobetu0-1tuoi800g_dd28e4aa93e54376b54bc080999738c0.png</v>
+      </c>
+      <c r="K2" t="str">
+        <v>MEIJI</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Sữa Meiji số 0 - 1 tuổi dạng hộp sắt có hương vị gần giống sữa mẹ, giúp bé dễ thích nghi, không chê ti mẹ cùng thành phần chất xơ tự nhiên tránh táo bón.</v>
+      </c>
+      <c r="M2">
+        <v>48500000</v>
+      </c>
+      <c r="N2">
+        <v>55500000</v>
+      </c>
+      <c r="O2" t="str">
+        <v>12.612612612612612%</v>
+      </c>
+      <c r="P2" t="str">
+        <v>&lt;h2 class="section-title text-blue"&gt;&lt;span style="color:#ff0066"&gt;&lt;strong&gt;Thông số sản phẩm&lt;/strong&gt;&lt;/span&gt;&lt;/h2&gt;&lt;div class="data-table"&gt;&lt;table&gt;&lt;tbody&gt;&lt;tr&gt;&lt;td&gt;&lt;span&gt;Sản phẩm&lt;/span&gt;&lt;/td&gt;&lt;td&gt;&lt;span&gt;Sữa Meiji số 0-1 tuổi&lt;/span&gt;&amp;nbsp;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;span&gt;Xuất xứ&lt;/span&gt;&lt;/td&gt;&lt;td&gt;&lt;span&gt;Nhật Bản&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;span&gt;Hãng sản xuất&lt;/span&gt;&lt;/td&gt;&lt;td&gt;&lt;span&gt;Meiji&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;span&gt;Trọng lượng&lt;/span&gt;&lt;/td&gt;&lt;td&gt;&lt;span&gt;800g&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;&lt;span&gt;Quy cách đóng gói&lt;/span&gt;&lt;/td&gt;&lt;td&gt;&lt;span&gt;Hộp sẳt&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;&lt;div&gt;&amp;nbsp;&lt;/div&gt;&lt;/div&gt;&lt;div class="section-title text-blue"&gt;&lt;strong&gt;Thông tin sản phẩm&lt;/strong&gt;&lt;/div&gt;&lt;div class="article-content show-hide-content"&gt;&lt;p&gt;&lt;strong&gt;Sữa Meiji số 0 - 1 tuổi dạng hộp sắt&lt;/strong&gt; là sữa bột công thức hàng đầu cho trẻ sơ sinh được các mẹ bỉm sữa nội địa Nhật và cả Việt Nam tin dùng. Bởi sữa Meiji số 0 có hương vị gần giống sữa mẹ, giúp bé dễ thích nghi với sữa bột, lại không chê ti mẹ. Đặc biệt, sữa có thành phần bổ sung chất xơ tự nhiên hạn chế bị táo bón hiệu quả.&lt;/p&gt;&lt;h2&gt;&lt;strong&gt;1. Thành phần dinh dưỡng sữa Meiji số 0&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;&lt;img alt="Bảng thành phần dinh dưỡng của sữa Meiji số 0" title="Bảng thành phần dinh dưỡng của sữa Meiji số 0" src="https://product.hstatic.net/200000833669/product/bang-dinh-duong-sua-meiji-so-0-1-tuoi_8e2ded54f4dc45559f2f45ecd320b440.jpg"&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Bảng dinh dưỡng sữa Meiji số 0 cho bé 0 - 12 tháng tuổi&lt;/em&gt;&lt;/p&gt;&lt;h2&gt;&lt;strong&gt;2. Thành phần nổi bật&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;Sữa Meiji số 0 hỗ trợ mẹ mang đến cho bé nguồn dinh dưỡng an toàn, đầy đủ để vững tin phát triển trong những năm tháng đầu đời. Cụ thể, sữa Meiji có những thành phần nổi bật đó là:&lt;/p&gt;&lt;h3&gt;Bổ sung chất xơ tự nhiên FOS (Fructo-Oligosaccharides)&lt;/h3&gt;&lt;p&gt;Các nghiên cứu cho thấy FOS là chất xơ hòa tan, có rất nhiều lợi ích đối với sức khỏe con người. Đây là người bạn tuyệt vời của hệ tiêu hóa, tim mạch, hệ miễn dịch,...&lt;/p&gt;&lt;h3&gt;Cung cấp nhiều vitamin và các khoáng chất thiết yếu&lt;/h3&gt;&lt;p&gt;Trong thành phần của sữa Meiji rất giàu vitamin như: A, C, D, vitamin nhóm B,... cùng các khoáng chất cần thiết (sắt, kẽm, photpho,...) hỗ trợ tối ưu sự phát triển toàn diện cho bé.&lt;/p&gt;&lt;h3&gt;Bổ sung các Nucleotides tự nhiên có trong sữa mẹ&lt;/h3&gt;&lt;p&gt;Meiji hiểu rằng ở giai đoạn đầu đời hệ miễn dịch của con còn rất non yếu, dễ bị vi khuẩn tấn công và nhiễm bệnh. Vì thế, công thức sữa cho trẻ sơ sinh của Meiji đã bổ sung thêm các Nucleotides tự nhiên có trong sữa mẹ giúp tăng cường đề kháng.&lt;/p&gt;&lt;p&gt;&lt;img src="https://product.hstatic.net/200000833669/product/se1bbafa-meiji-0-2_16b8a8ff0726471c9a9833f51053862b.jpg"&gt;&lt;img src="https://product.hstatic.net/200000833669/product/se1bbafa-meiji-0_3da58f5faf6c4823b559a5d1ecdd4674.jpg"&gt;&lt;/p&gt;&lt;div&gt;&lt;div class="ace-line ace-line old-record-id-WDu1dC4sBowBjSxZhEDlYiHSgrh"&gt;&lt;em&gt;Thiết kế bao bì dễ sử dụng của sữa Meiji số 0 nội địa Nhật&lt;/em&gt;&lt;/div&gt;&lt;/div&gt;&lt;h2&gt;&lt;strong&gt;3. Đặc điểm nổi bật của sữa Meiji số 0&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;Cẩm nang nuôi con khỏe mạnh - thông minh của nhiều mẹ bỉm sữa chia sẻ thường dành nhiều lời khen ngợi cho sữa Meiji số 0. Bởi sản phẩm có những đặc điểm nổi bật mà mẹ rất tâm đắc, cụ thể:&lt;/p&gt;&lt;h3&gt;Sữa có vị nhạt, mùi vị gần giống sữa mẹ&lt;/h3&gt;&lt;p&gt;Các mẹ thường có một nỗi lo lắng chung là sữa công thức thơm ngon hơn sữa mẹ, dễ khiến bé chê ti mẹ. Trong khi đó, sữa mẹ luôn là nguồn dinh dưỡng tốt nhất cho sự phát triển của trẻ sơ sinh và trẻ nhỏ. Hiểu được điều đó, sữa Meiji số 0 đã ra đời với hương thơm cùng mùi vị gần giống sữa mẹ nhất. Do vậy, mẹ cứ yên tâm sử dụng cả sữa mẹ lẫn sữa công thức cho bé nhé!&lt;/p&gt;&lt;h3&gt;Hỗ trợ bé tăng cân, chiều cao đều, không tăng nhanh, tránh béo phì&lt;/h3&gt;&lt;p&gt;Với thành phần dinh dưỡng cân bằng, hướng tới sự phát triển toàn diện, sữa Meiji số 0 là người bạn đồng hành lý tưởng hỗ trợ bé tăng cân và chiều cao đồng đều. Nhờ vậy, mẹ chẳng lo con bị béo phì, thừa cân mà có thể yên tâm nhìn con cao lớn từng chút một khỏe mạnh và ổn định.&lt;/p&gt;&lt;p&gt;&lt;img alt="Sữa Meiji số 0 giúp bé hạn chế táo bón" title="Sữa Meiji số 0 giúp bé hạn chế táo bón" src="https://product.hstatic.net/200000833669/product/sua-meiji-so-0-giup-be-han-che-tao-bon_ba6b62df8c574dacbd09e603cbf5624c.jpg"&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Với sữa Meiji số 0 mẹ có thể an tâm con tiêu hóa tốt, ít bị táo bón&lt;span&gt;&amp;nbsp;&lt;/span&gt;&lt;/em&gt;&lt;/p&gt;&lt;h3&gt;Hạn chế táo bón, phân xốp cùng hệ tiêu hóa khỏe mạnh&lt;/h3&gt;&lt;p&gt;Sữa Meiji giúp bé củng cố sức khỏe đường ruột, tiêu hóa tốt hơn nhờ có thành phần chất xơ tự nhiên FOS. Bởi khi vào ruột, FOS sẽ hút nước trương nở tạo khối phân, làm mềm phân và giúp đào thải phân cùng các chất cặn bã nhanh chóng ra khỏi cơ thể.&lt;/p&gt;&lt;p&gt;Bên cạnh đó, FOS còn có tác dụng&lt;strong&gt; kích thích các lợi khuẩn trong đường ruột phát triển&lt;/strong&gt;, đồng thời giúp tăng cường hấp thu canxi cùng magie tại ruột già. Vì thế, bé uống sữa Meiji mẹ yên tâm lắm bởi bé ít bị táo bón và hấp thu dưỡng chất tốt hơn.&lt;/p&gt;&lt;h3&gt;Tăng cường sức đề kháng, nâng cao miễn dịch&lt;/h3&gt;&lt;p&gt;Chất xơ hòa tan FOS cùng với &lt;strong&gt;các Nucleotides tự nhiên&lt;/strong&gt; trong sữa Meiji có khả năng tăng cường miễn dịch, cho bé sức đề kháng tốt để chống chọi với vi khuẩn, bệnh tật.&lt;/p&gt;&lt;h2&gt;&lt;strong&gt;4. Hướng dẫn cách pha sữa Meiji số 0&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;Nhiều mẹ bỉm sữa, nhất là những chị em làm mẹ lần đầu rất lúng túng trong việc pha sữa Meiji cho bé. Mẹ không biết 1 gạt thìa sữa pha khoảng bao nhiêu ml thì hợp lý. Dưới đây là hướng dẫn cách pha chuẩn theo hướng dẫn của nhà sản xuất các mẹ cần biết:&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Một thìa gạt ngang&lt;/strong&gt; sữa Meiji tương đương 2,7g bột sữa pha được&lt;strong&gt; 20ml sữa.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Cách pha:&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bước 1: Đầu tiên, bố mẹ cần đun sôi dụng cụ pha sữa trong vòng&lt;strong&gt; 3 - 5 phút&lt;/strong&gt; để khử trùng.&lt;/li&gt;&lt;li&gt;Bước 2: Lấy nước sôi&lt;strong&gt; để&lt;/strong&gt; &lt;strong&gt;nguội đến 70 độ C&lt;/strong&gt; pha sữa.&lt;/li&gt;&lt;li&gt;Bước 3: Sử dụng thìa lấy sữa chuyên dụng trong hộp để lấy chính xác lượng sữa cần pha. Cho sữa vào dụng cụ pha rồi đổ vào &lt;strong&gt;⅔ lượng nước cần thiết&lt;/strong&gt; và lắc/ khuấy đều đến khi hòa tan sữa. (Do nước ở 70 độ C khá nóng nên bố mẹ cần cẩn thận tránh bị bỏng).&lt;/li&gt;&lt;li&gt;Bước 4: Đổ tiếp nước 70 độ vào bình cho đủ lượng nước theo chỉ định và tiếp tục lắc/ khuấy đều.&lt;/li&gt;&lt;li&gt;Bước 5: Chờ sữa nguội khoảng &lt;strong&gt;38 độ C&lt;/strong&gt; thì cho bé bú.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Tham khảo:&amp;nbsp;&lt;a style="font-family: -apple-system, BlinkMacSystemFont, 'Segoe UI', Roboto, 'Helvetica Neue', Arial, 'Noto Sans', sans-serif, 'Apple Color Emoji', 'Segoe UI Emoji', 'Segoe UI Symbol', 'Noto Color Emoji'; font-size: 1.25rem; font-weight: 700; background-color: #ffffff; text-align: left;" href="/blogs/me-be/huong-dan-cach-pha-sua-meiji-so-0-9-chuan"&gt;&lt;span&gt;[HƯỚNG DẪN] Cách pha sữa Meiji số 0, 9 chuẩn hướng dẫn Nhà sản xuất&lt;/span&gt;&lt;/a&gt;&lt;/p&gt;&lt;div style="outline: 0px; vertical-align: baseline; margin: 0px; border-width: 0px 0px 1px; border-top-style: initial; border-right-style: initial; border-bottom-style: solid; border-left-style: initial; border-top-color: initial; border-right-color: initial; border-bottom-color: #ebebeb; border-left-color: initial; border-image: initial; padding: 0px 0px 15px; font-variant-numeric: inherit; font-variant-east-asian: inherit; font-variant-alternates: inherit; font-variant-position: inherit; font-stretch: inherit; line-height: inherit; font-family: -apple-system, BlinkMacSystemFont, 'Segoe UI', Roboto, 'Helvetica Neue', Arial, 'Noto Sans', sans-serif, 'Apple Color Emoji', 'Segoe UI Emoji', 'Segoe UI Symbol', 'Noto Color Emoji'; font-optical-sizing: inherit; font-kerning: inherit; font-feature-settings: inherit; font-variation-settings: inherit; display: flex; -webkit-box-pack: justify; justify-content: space-between; -webkit-box-align: center; align-items: center; color: #333333;" class="news-detail-meta flex justify-between items-center"&gt;&amp;nbsp;&lt;/div&gt;&lt;p&gt;&lt;img alt="Pha sữa Meiji số 0 dùng nước 70 độ " title="Pha sữa Meiji số 0 dùng nước 70 độ " src="https://product.hstatic.net/200000833669/product/pha-sua-meiji-so-0_6192ae5cb53d48f7ac4e3ab0b0c52cb4.jpg"&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Sữa Meiji số 0 khác với các loại sữa Nhật khác là sử dụng nước pha ở 70 độ C&lt;span&gt;&amp;nbsp;&lt;/span&gt;&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Mẹo khi pha sữa:&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Mẹ có thể&lt;strong&gt; cho bình sữa vào chậu nước mát, lạnh&lt;/strong&gt; để nguội nhanh hơn, tiết kiệm thời gian.&lt;/li&gt;&lt;li&gt;Trước khi cho bé bú, mẹ hãy &lt;strong&gt;kiểm tra nhiệt độ của sữa&lt;/strong&gt; tránh làm bỏng bé.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;Liều lượng sữa cho bé theo từng độ tuổi:&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;img alt="Liều lượng sữa Meiji số 0 cho bé theo độ tuổi" title="Liều lượng sữa Meiji số 0 cho bé theo độ tuổi" src="https://product.hstatic.net/200000833669/product/lieu-luong-sua-meiji-so-0-theo-do-tuoi-cua-be_5ed9bd72449947e3bd19ac0f1138e626.jpg"&gt;&lt;/p&gt;&lt;p&gt;&lt;span&gt;&lt;em&gt;Tùy độ tuổi, cân nặng của bé mà mẹ sử dụng lượng sữa khác nhau&lt;/em&gt;&lt;/span&gt;&lt;span&gt;&lt;em&gt;&amp;nbsp;&lt;/em&gt;&lt;/span&gt;&lt;/p&gt;&lt;h2&gt;&lt;strong&gt;5. Hướng dẫn bảo quản&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;Mẹ cần chú ý bảo quản sữa đúng cách như sau:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bảo quản sữa Meiji ở những nơi khô thoáng&lt;/li&gt;&lt;li&gt;Tránh sự tiếp xúc với ánh nắng trực tiếp, những nơi có nhiệt độ cao hoặc ẩm ướt&lt;/li&gt;&lt;li&gt;Sữa Meiji đã pha có thời gian sử dụng là 2 tiếng sau khi pha và chỉ dùng 1 lần. Nếu bé uống không hết, còn thừa mẹ cũng tuyệt đối không cho bé dùng tiếp.&lt;/li&gt;&lt;li&gt;Hạn sử dụng của sữa được in dưới đáy lon là 18 tháng kể từ ngày sản xuất.&lt;/li&gt;&lt;li&gt;Đóng nắp sữa thật chặt sau mỗi lần lấy và chỉ nên sử dụng trong khoảng 30 ngày kể từ khi mở nắp hộp để đảm bảo chất lượng sữa tốt nhất. Sau 30 ngày sữa còn mẹ cũng có thể dụng nhưng chất lượng không bằng ban đầu.&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;&lt;strong&gt;6. Thông tin thương hiệu sữa Meiji&lt;/strong&gt;&lt;/h2&gt;&lt;p&gt;Sữa Meiji là sản phẩm của công ty Meiji thuộc tập đoàn Meiji Holdings Co., Ltd được thành lập vào năm 1917. Với tuổi đời hơn 100 năm, cái tên Meiji đã trở thành một trong những thương hiệu sữa truyền thống hàng đầu không chỉ ở Nhật Bản mà cả Châu Á. Các sản phẩm sữa của hãng luôn đảm bảo chất lượng tốt, đạt chứng nhận ISO 9001 được người dùng tại nhiều nước trên thế giới tin dùng.&lt;/p&gt;&lt;p&gt;Hiện Meiji cung cấp hơn 4000 mặt hàng với 6 dòng sản phẩm chính, chủ yếu là sản phẩm từ sữa. Trong đó, sữa bột, sữa chua,... chiếm thị phần số 1 ở thị trường nội địa Nhật.&lt;/p&gt;&lt;p&gt;Tại Việt Nam, sữa Meiji cũng nhận được nhiều đánh giá, review tốt của các mẹ bỉm sữa. Với chất lượng đảm bảo, tốt cho sự phát triển của bé và mức giá không quá cao, &lt;strong&gt;sữa Meiji số 0 - 1 tuổi dạng hộp sắt&lt;/strong&gt; vẫn luôn là sự lựa chọn hàng đầu cho giai đoạn đầu đời của bé.&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:P2"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add scrape in category
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -19,6 +19,8 @@
     <sheet name="all1726463533607" sheetId="14" r:id="rId14"/>
     <sheet name="sua-cho-be1726464944601" sheetId="15" r:id="rId15"/>
     <sheet name="all1726464945050" sheetId="16" r:id="rId16"/>
+    <sheet name="sua-cho-be1726495628346" sheetId="17" r:id="rId17"/>
+    <sheet name="all1726495628544" sheetId="18" r:id="rId18"/>
   </sheets>
 </workbook>
 </file>
@@ -1797,6 +1799,284 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>url</v>
+      </c>
+      <c r="C1" t="str">
+        <v>title</v>
+      </c>
+      <c r="D1" t="str">
+        <v>type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>inventoryQuantity</v>
+      </c>
+      <c r="F1" t="str">
+        <v>inventoryPolicy</v>
+      </c>
+      <c r="G1" t="str">
+        <v>sku</v>
+      </c>
+      <c r="H1" t="str">
+        <v>barcode</v>
+      </c>
+      <c r="I1" t="str">
+        <v>featuredImage</v>
+      </c>
+      <c r="J1" t="str">
+        <v>images</v>
+      </c>
+      <c r="K1" t="str">
+        <v>trademark</v>
+      </c>
+      <c r="L1" t="str">
+        <v>shortDescription</v>
+      </c>
+      <c r="M1" t="str">
+        <v>price</v>
+      </c>
+      <c r="N1" t="str">
+        <v>originalPrice</v>
+      </c>
+      <c r="O1" t="str">
+        <v>percentDiscount</v>
+      </c>
+      <c r="P1" t="str">
+        <v>description</v>
+      </c>
+    </row>
+    <row r="2" xml:space="preserve">
+      <c r="A2">
+        <v>1052912101</v>
+      </c>
+      <c r="B2" t="str">
+        <v>https://sakukostore.com.vn/products/kumano-yushi-gel-dung-chiet-xuat-mat-ong-300g</v>
+      </c>
+      <c r="C2" t="str">
+        <v>KUMANO YUSHI- Gel dưỡng chiết xuất mật ong (300g)</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Kem dưỡng</v>
+      </c>
+      <c r="E2">
+        <v>18</v>
+      </c>
+      <c r="F2" t="str">
+        <v>continue</v>
+      </c>
+      <c r="G2" t="str">
+        <v>101780</v>
+      </c>
+      <c r="H2" t="str">
+        <v>4513574037847</v>
+      </c>
+      <c r="I2" t="str">
+        <v>https://product.hstatic.net/200000833669/product/4513574037847_66bbbb8f6ad04d79ae7f988e6fdd0294.jpg</v>
+      </c>
+      <c r="J2" t="str">
+        <v>https://product.hstatic.net/200000833669/product/4513574037847_66bbbb8f6ad04d79ae7f988e6fdd0294.jpg</v>
+      </c>
+      <c r="K2" t="str">
+        <v>KUMANOYUSHI</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Dưỡng ẩm an toàn với thành phần thiên nhiên  Bổ sung collagen và ceramide chống lão hóa  Công thức dưỡng ẩm 5 trong 1 tiện lợi</v>
+      </c>
+      <c r="M2">
+        <v>18900000</v>
+      </c>
+      <c r="N2">
+        <v>18900000</v>
+      </c>
+      <c r="O2" t="str">
+        <v>0%</v>
+      </c>
+      <c r="P2" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;h2 class="section-title text-blue"&gt;Thông tin chi tiết&lt;/h2&gt;&lt;div class="section-title text-blue"&gt;Thông tin sản phẩm&lt;/div&gt; &lt;div class="article-content show-hide-content"&gt;&lt;p&gt;&lt;strong&gt;Gel dưỡng ẩm Deve Honey Manuka&lt;/strong&gt; giàu dưỡng chất dưỡng da và tính kháng khuẩn cao với thành phần chính là dưỡng chất mật ong, collagen và ceramide. Sản phẩm giúp cấp ẩm sâu, làm chậm quá trình lão hóa, đồng thời kháng khuẩn, chống viêm, giảm thiểu tình trạng mụn và thâm sau mụn hiệu quả.&lt;/p&gt;
+   &lt;h2&gt;THÀNH PHẦN&lt;/h2&gt;
+   &lt;p&gt;Water, Glycerin, Butylene Glycol, dưỡng chất mật ong, Soluble Collagen, Sodium Hyaluronate, Arginine, Ceramide NG, hương liệu và các thành phần khác.&lt;/p&gt;
+   &lt;h2&gt;QUY CÁCH ĐÓNG GÓI&lt;/h2&gt;
+   &lt;p&gt;Hũ 300g&lt;/p&gt;
+   &lt;p&gt;&lt;img src="https://product.hstatic.net/200000833669/product/ng-e1baa9m-deve-honey-manuka-dc6b0e1bba1ng-che1baa5t-me1baadt-ong-300g_0c70e959a79847cfa3a61c0f46d1d941.jpg" alt="KUMANO YUSHI- Gel dưỡng ẩm Deve Honey Manuka dưỡng chất mật ong (300g)" title="KUMANO YUSHI- Gel dưỡng ẩm Deve Honey Manuka dưỡng chất mật ong (300g)"&gt;&lt;br&gt;
+   Gel dưỡng ẩm 5 trong 1 dưỡng chất mật ong dưỡng ẩm sâu, chống viêm, kháng khuẩn, ngăn ngừa mụn và thâm mụn&lt;/p&gt;
+   &lt;h2&gt;CÔNG DỤNG&lt;/h2&gt;
+   &lt;h3&gt;Dưỡng ẩm an toàn với thành phần thiên nhiên&lt;/h3&gt;
+   &lt;p&gt;Gel dưỡng Deve Honey Manuka chứa thành phần mật ong cung cấp nước tạo độ ẩm cho da. Đồng thời, mật ong có khả năng kháng khuẩn, làm dịu vùng da bị tổn thương và hỗ trợ giảm thâm mụn hiệu quả&lt;/p&gt;
+   &lt;h3&gt;Bổ sung collagen và ceramide chống lão hóa&lt;/h3&gt;
+   &lt;p&gt;Sản phẩm được bổ sung thêm thành phần collagen giúp tăng độ săn chắc và đàn hồi, cải thiện các tình trạng lão hóa da như khô ráp, thâm nám và phục hồi làn da bị tổn thương do mụn. Bên cạnh đó, ceramide bảo vệ lớp biểu bì trước các tác hại của môi trường và chống lão hóa nhờ khả năng dưỡng ẩm hiệu quả&lt;/p&gt;
+   &lt;h3&gt;Công thức dưỡng ẩm 5 trong 1 tiện lợi khi chăm sóc da&lt;/h3&gt;
+   &lt;p&gt;Sản phẩm được nghiên cứu, sản xuất dựa trên công thức 5in1 gồm: Nước hoa hồng, sữa dưỡng, kem dưỡng, serum, mặt nạ, giúp đơn giản hóa các bước chăm sóc da chỉ trong một sản phẩm.&amp;nbsp;&lt;/p&gt;
+   &lt;h2&gt;HƯỚNG DẪN SỬ DỤNG&lt;/h2&gt;
+   &lt;ul&gt; &lt;li&gt;Sử dụng trên nền da khô.&amp;nbsp;&lt;/li&gt; &lt;li&gt;Thoa một lượng vừa đủ lên da, đặc biệt tại các vùng da khô cần chăm sóc.&amp;nbsp;&lt;/li&gt; &lt;li&gt;Có thể sử dụng dưỡng da toàn thân.&lt;/li&gt;
+   &lt;/ul&gt;
+   &lt;h2&gt;LƯU Ý&amp;nbsp;&lt;/h2&gt;
+   &lt;ul&gt; &lt;li&gt;Không sử dụng nếu dị ứng với bất kì thành phần nào của sản phẩm.&amp;nbsp;&lt;/li&gt; &lt;li&gt;Ngưng sử dụng khi có triệu chứng bất thường.&lt;/li&gt;
+   &lt;/ul&gt;
+   &lt;h2&gt;BẢO QUẢN&lt;/h2&gt;
+   &lt;ul&gt; &lt;li&gt;Nơi khô thoáng, tránh ánh nắng mặt trời trực tiếp.&amp;nbsp;&lt;/li&gt; &lt;li&gt;Để xa tầm tay trẻ em.&lt;/li&gt;
+   &lt;/ul&gt;
+   &lt;h2&gt;THƯƠNG HIỆU&lt;/h2&gt;
+   &lt;p&gt;Gel dưỡng ẩm Deve Honey Manuka được sản xuất bởi Kumanoyushi Co.,Ltd. 35 Kumano-Cho, Seto-shi, Aichi, Nhật Bản. Kumanoyushi là công ty sản xuất mỹ phẩm được thành lập vào năm 1952 tại Nhật Bản. Với mục tiêu tạo ra những sản phẩm chiết xuất từ thiên nhiên tốt nhất cho làn da, thân thiện với sức khỏe, Kumanoyushi nhận được sự tin cậy của người tiêu dùng không chỉ tại Nhật Bản mà tại nhiều quốc gia khác, trong đó có Việt Nam.&lt;br&gt;
+   &lt;strong&gt;Gel dưỡng ẩm Deve Honey Manuka&lt;/strong&gt; hiện đã có sẵn trên các kệ hàng của Sakuko Japanese Store, hệ thống siêu thị hàng nội địa Nhật Bản chính hãng sẵn sàng tư vấn và giải đáp mọi thắc mắc. Mời bạn liên hệ ngay với chúng tôi.&amp;nbsp;&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:P2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>url</v>
+      </c>
+      <c r="C1" t="str">
+        <v>title</v>
+      </c>
+      <c r="D1" t="str">
+        <v>type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>inventoryQuantity</v>
+      </c>
+      <c r="F1" t="str">
+        <v>inventoryPolicy</v>
+      </c>
+      <c r="G1" t="str">
+        <v>sku</v>
+      </c>
+      <c r="H1" t="str">
+        <v>barcode</v>
+      </c>
+      <c r="I1" t="str">
+        <v>featuredImage</v>
+      </c>
+      <c r="J1" t="str">
+        <v>images</v>
+      </c>
+      <c r="K1" t="str">
+        <v>trademark</v>
+      </c>
+      <c r="L1" t="str">
+        <v>shortDescription</v>
+      </c>
+      <c r="M1" t="str">
+        <v>price</v>
+      </c>
+      <c r="N1" t="str">
+        <v>originalPrice</v>
+      </c>
+      <c r="O1" t="str">
+        <v>percentDiscount</v>
+      </c>
+      <c r="P1" t="str">
+        <v>description</v>
+      </c>
+    </row>
+    <row r="2" xml:space="preserve">
+      <c r="A2">
+        <v>1052912101</v>
+      </c>
+      <c r="B2" t="str">
+        <v>https://sakukostore.com.vn/products/kumano-yushi-gel-dung-chiet-xuat-mat-ong-300g</v>
+      </c>
+      <c r="C2" t="str">
+        <v>KUMANO YUSHI- Gel dưỡng chiết xuất mật ong (300g)</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Kem dưỡng</v>
+      </c>
+      <c r="E2">
+        <v>18</v>
+      </c>
+      <c r="F2" t="str">
+        <v>continue</v>
+      </c>
+      <c r="G2" t="str">
+        <v>101780</v>
+      </c>
+      <c r="H2" t="str">
+        <v>4513574037847</v>
+      </c>
+      <c r="I2" t="str">
+        <v>https://product.hstatic.net/200000833669/product/4513574037847_66bbbb8f6ad04d79ae7f988e6fdd0294.jpg</v>
+      </c>
+      <c r="J2" t="str">
+        <v>https://product.hstatic.net/200000833669/product/4513574037847_66bbbb8f6ad04d79ae7f988e6fdd0294.jpg</v>
+      </c>
+      <c r="K2" t="str">
+        <v>KUMANOYUSHI</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Dưỡng ẩm an toàn với thành phần thiên nhiên  Bổ sung collagen và ceramide chống lão hóa  Công thức dưỡng ẩm 5 trong 1 tiện lợi</v>
+      </c>
+      <c r="M2">
+        <v>18900000</v>
+      </c>
+      <c r="N2">
+        <v>18900000</v>
+      </c>
+      <c r="O2" t="str">
+        <v>0%</v>
+      </c>
+      <c r="P2" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;h2 class="section-title text-blue"&gt;Thông tin chi tiết&lt;/h2&gt;&lt;div class="section-title text-blue"&gt;Thông tin sản phẩm&lt;/div&gt; &lt;div class="article-content show-hide-content"&gt;&lt;p&gt;&lt;strong&gt;Gel dưỡng ẩm Deve Honey Manuka&lt;/strong&gt; giàu dưỡng chất dưỡng da và tính kháng khuẩn cao với thành phần chính là dưỡng chất mật ong, collagen và ceramide. Sản phẩm giúp cấp ẩm sâu, làm chậm quá trình lão hóa, đồng thời kháng khuẩn, chống viêm, giảm thiểu tình trạng mụn và thâm sau mụn hiệu quả.&lt;/p&gt;
+   &lt;h2&gt;THÀNH PHẦN&lt;/h2&gt;
+   &lt;p&gt;Water, Glycerin, Butylene Glycol, dưỡng chất mật ong, Soluble Collagen, Sodium Hyaluronate, Arginine, Ceramide NG, hương liệu và các thành phần khác.&lt;/p&gt;
+   &lt;h2&gt;QUY CÁCH ĐÓNG GÓI&lt;/h2&gt;
+   &lt;p&gt;Hũ 300g&lt;/p&gt;
+   &lt;p&gt;&lt;img src="https://product.hstatic.net/200000833669/product/ng-e1baa9m-deve-honey-manuka-dc6b0e1bba1ng-che1baa5t-me1baadt-ong-300g_0c70e959a79847cfa3a61c0f46d1d941.jpg" alt="KUMANO YUSHI- Gel dưỡng ẩm Deve Honey Manuka dưỡng chất mật ong (300g)" title="KUMANO YUSHI- Gel dưỡng ẩm Deve Honey Manuka dưỡng chất mật ong (300g)"&gt;&lt;br&gt;
+   Gel dưỡng ẩm 5 trong 1 dưỡng chất mật ong dưỡng ẩm sâu, chống viêm, kháng khuẩn, ngăn ngừa mụn và thâm mụn&lt;/p&gt;
+   &lt;h2&gt;CÔNG DỤNG&lt;/h2&gt;
+   &lt;h3&gt;Dưỡng ẩm an toàn với thành phần thiên nhiên&lt;/h3&gt;
+   &lt;p&gt;Gel dưỡng Deve Honey Manuka chứa thành phần mật ong cung cấp nước tạo độ ẩm cho da. Đồng thời, mật ong có khả năng kháng khuẩn, làm dịu vùng da bị tổn thương và hỗ trợ giảm thâm mụn hiệu quả&lt;/p&gt;
+   &lt;h3&gt;Bổ sung collagen và ceramide chống lão hóa&lt;/h3&gt;
+   &lt;p&gt;Sản phẩm được bổ sung thêm thành phần collagen giúp tăng độ săn chắc và đàn hồi, cải thiện các tình trạng lão hóa da như khô ráp, thâm nám và phục hồi làn da bị tổn thương do mụn. Bên cạnh đó, ceramide bảo vệ lớp biểu bì trước các tác hại của môi trường và chống lão hóa nhờ khả năng dưỡng ẩm hiệu quả&lt;/p&gt;
+   &lt;h3&gt;Công thức dưỡng ẩm 5 trong 1 tiện lợi khi chăm sóc da&lt;/h3&gt;
+   &lt;p&gt;Sản phẩm được nghiên cứu, sản xuất dựa trên công thức 5in1 gồm: Nước hoa hồng, sữa dưỡng, kem dưỡng, serum, mặt nạ, giúp đơn giản hóa các bước chăm sóc da chỉ trong một sản phẩm.&amp;nbsp;&lt;/p&gt;
+   &lt;h2&gt;HƯỚNG DẪN SỬ DỤNG&lt;/h2&gt;
+   &lt;ul&gt; &lt;li&gt;Sử dụng trên nền da khô.&amp;nbsp;&lt;/li&gt; &lt;li&gt;Thoa một lượng vừa đủ lên da, đặc biệt tại các vùng da khô cần chăm sóc.&amp;nbsp;&lt;/li&gt; &lt;li&gt;Có thể sử dụng dưỡng da toàn thân.&lt;/li&gt;
+   &lt;/ul&gt;
+   &lt;h2&gt;LƯU Ý&amp;nbsp;&lt;/h2&gt;
+   &lt;ul&gt; &lt;li&gt;Không sử dụng nếu dị ứng với bất kì thành phần nào của sản phẩm.&amp;nbsp;&lt;/li&gt; &lt;li&gt;Ngưng sử dụng khi có triệu chứng bất thường.&lt;/li&gt;
+   &lt;/ul&gt;
+   &lt;h2&gt;BẢO QUẢN&lt;/h2&gt;
+   &lt;ul&gt; &lt;li&gt;Nơi khô thoáng, tránh ánh nắng mặt trời trực tiếp.&amp;nbsp;&lt;/li&gt; &lt;li&gt;Để xa tầm tay trẻ em.&lt;/li&gt;
+   &lt;/ul&gt;
+   &lt;h2&gt;THƯƠNG HIỆU&lt;/h2&gt;
+   &lt;p&gt;Gel dưỡng ẩm Deve Honey Manuka được sản xuất bởi Kumanoyushi Co.,Ltd. 35 Kumano-Cho, Seto-shi, Aichi, Nhật Bản. Kumanoyushi là công ty sản xuất mỹ phẩm được thành lập vào năm 1952 tại Nhật Bản. Với mục tiêu tạo ra những sản phẩm chiết xuất từ thiên nhiên tốt nhất cho làn da, thân thiện với sức khỏe, Kumanoyushi nhận được sự tin cậy của người tiêu dùng không chỉ tại Nhật Bản mà tại nhiều quốc gia khác, trong đó có Việt Nam.&lt;br&gt;
+   &lt;strong&gt;Gel dưỡng ẩm Deve Honey Manuka&lt;/strong&gt; hiện đã có sẵn trên các kệ hàng của Sakuko Japanese Store, hệ thống siêu thị hàng nội địa Nhật Bản chính hãng sẵn sàng tư vấn và giải đáp mọi thắc mắc. Mời bạn liên hệ ngay với chúng tôi.&amp;nbsp;&lt;/p&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:P2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P9"/>

</xml_diff>